<commit_message>
added more aircraft data
</commit_message>
<xml_diff>
--- a/ReferenceAircraft.xlsx
+++ b/ReferenceAircraft.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owenm\Projects\DSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owenm\Projects\DSE\Ekranoplan-DSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BDA2A0-31DD-4D43-BF55-8FC086A23498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D492C0DC-4C7F-40DF-82AD-ADFBBF5CC85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>FS40</t>
+  </si>
+  <si>
+    <t>C-130</t>
+  </si>
+  <si>
+    <t>C-17</t>
+  </si>
+  <si>
+    <t>C-5</t>
+  </si>
+  <si>
+    <t>Convair</t>
+  </si>
+  <si>
+    <t>Hughes</t>
   </si>
 </sst>
 </file>
@@ -430,10 +445,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,6 +561,61 @@
         <v>20900</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>34686</v>
+      </c>
+      <c r="C11" s="1">
+        <v>70305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>128140</v>
+      </c>
+      <c r="C12" s="1">
+        <v>265352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>169640</v>
+      </c>
+      <c r="C13" s="1">
+        <v>379655</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>32579</v>
+      </c>
+      <c r="C14" s="1">
+        <v>74843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>122500</v>
+      </c>
+      <c r="C15" s="1">
+        <v>181500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>